<commit_message>
auto open url and screenshot
</commit_message>
<xml_diff>
--- a/3.xlsx
+++ b/3.xlsx
@@ -14,32 +14,524 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="179">
+  <si>
+    <t>Story Number</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Outlet Name</t>
+  </si>
+  <si>
+    <t>Media Type</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Source Type</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Potential Audience</t>
+  </si>
+  <si>
+    <t>Unnamed: 9</t>
+  </si>
+  <si>
+    <t>Unnamed: 10</t>
+  </si>
+  <si>
+    <t>Headline</t>
+  </si>
   <si>
     <t>FR34887</t>
   </si>
   <si>
+    <t>EN34887</t>
+  </si>
+  <si>
+    <t>GE34887</t>
+  </si>
+  <si>
+    <t>SP34887</t>
+  </si>
+  <si>
+    <t>Tweets</t>
+  </si>
+  <si>
+    <t>Twitter Handle</t>
+  </si>
+  <si>
+    <t>Newswire IO (newswireio)</t>
+  </si>
+  <si>
+    <t>CIAR GLOBAL (CIAR_Global)</t>
+  </si>
+  <si>
+    <t>CentroIberoamericano (CIAR_Arbitraje)</t>
+  </si>
+  <si>
+    <t>Bojami Nguyen (NguyenBojami)</t>
+  </si>
+  <si>
+    <t>David Nguyen (davidvietnguyen)</t>
+  </si>
+  <si>
     <t>French</t>
   </si>
   <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>German</t>
+  </si>
+  <si>
+    <t>Spanish</t>
+  </si>
+  <si>
+    <t>https://twitter.com/newswireio/statuses/748462216266059776</t>
+  </si>
+  <si>
+    <t>https://twitter.com/CIAR_Global/statuses/748829787549011968</t>
+  </si>
+  <si>
+    <t>https://twitter.com/CIAR_Arbitraje/statuses/748834819207987200</t>
+  </si>
+  <si>
+    <t>https://twitter.com/NguyenBojami/statuses/748124799306731520</t>
+  </si>
+  <si>
+    <t>https://twitter.com/davidvietnguyen/statuses/748136832228024320</t>
+  </si>
+  <si>
     <t>World is Magiiic</t>
   </si>
   <si>
+    <t>wallstreet:online</t>
+  </si>
+  <si>
+    <t>Telegraph India</t>
+  </si>
+  <si>
+    <t>SurveySam.com</t>
+  </si>
+  <si>
+    <t>Stocklink</t>
+  </si>
+  <si>
+    <t>Pressemeldungen</t>
+  </si>
+  <si>
+    <t>Press-Release.by</t>
+  </si>
+  <si>
+    <t>PR Newswire UK</t>
+  </si>
+  <si>
+    <t>PR Newswire Sweden</t>
+  </si>
+  <si>
+    <t>PR Newswire France</t>
+  </si>
+  <si>
+    <t>PR Newswire</t>
+  </si>
+  <si>
+    <t>Padova News</t>
+  </si>
+  <si>
+    <t>One News Page United Kingdom Edition</t>
+  </si>
+  <si>
+    <t>One News Page Global Edition</t>
+  </si>
+  <si>
+    <t>news aktuell Switzerland</t>
+  </si>
+  <si>
+    <t>Netherlands Corporate News</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mokanews	</t>
+  </si>
+  <si>
+    <t>Mediaddress.es</t>
+  </si>
+  <si>
+    <t>Luso Financial Planning</t>
+  </si>
+  <si>
+    <t>Infrosoft</t>
+  </si>
+  <si>
+    <t>Global Newsweek</t>
+  </si>
+  <si>
+    <t>Finanznavigator</t>
+  </si>
+  <si>
+    <t>FinanzNachrichten.de (ABC New Media AG)</t>
+  </si>
+  <si>
+    <t>finanzen.net</t>
+  </si>
+  <si>
+    <t>Finanzen.at</t>
+  </si>
+  <si>
+    <t>EZERINCOM</t>
+  </si>
+  <si>
+    <t>Europa Press</t>
+  </si>
+  <si>
+    <t>ErDesvan</t>
+  </si>
+  <si>
+    <t>Diario de Leon</t>
+  </si>
+  <si>
+    <t>Der Tagesspiegel</t>
+  </si>
+  <si>
+    <t>Creditmarket.co.uk</t>
+  </si>
+  <si>
+    <t>Collaboration Technologies</t>
+  </si>
+  <si>
+    <t>BoxTicker.com</t>
+  </si>
+  <si>
+    <t>Boursica</t>
+  </si>
+  <si>
+    <t>Borse Social Network</t>
+  </si>
+  <si>
+    <t>BoerseGo</t>
+  </si>
+  <si>
+    <t>Belga Direct</t>
+  </si>
+  <si>
+    <t>B Live News</t>
+  </si>
+  <si>
+    <t>AssignmentEditor.com</t>
+  </si>
+  <si>
+    <t>Al-Adnani</t>
+  </si>
+  <si>
+    <t>ADVFN Mexico</t>
+  </si>
+  <si>
+    <t>ADVFN Germany</t>
+  </si>
+  <si>
+    <t>ADVFN France</t>
+  </si>
+  <si>
+    <t>ADN Kronos</t>
+  </si>
+  <si>
+    <t>2925 followers</t>
+  </si>
+  <si>
+    <t>88 followers</t>
+  </si>
+  <si>
+    <t>64 followers</t>
+  </si>
+  <si>
+    <t>33 followers</t>
+  </si>
+  <si>
+    <t>20 followers</t>
+  </si>
+  <si>
     <t>Online</t>
   </si>
   <si>
+    <t>Published on</t>
+  </si>
+  <si>
+    <t>2016-06-30 10:37:26</t>
+  </si>
+  <si>
+    <t>2016-07-01 10:52:25</t>
+  </si>
+  <si>
+    <t>2016-07-01 11:07:26</t>
+  </si>
+  <si>
+    <t>2016-06-29 12:07:36</t>
+  </si>
+  <si>
+    <t>2016-06-29 12:52:47</t>
+  </si>
+  <si>
     <t>http://worldismagiiic.blogspot.fr/p/magiiical-news.html?rkey=20160630FR34887&amp;filter=2987</t>
   </si>
   <si>
+    <t>http://www.wallstreet-online.de/nachricht/8721253-international-experts-question-proceedings-of-south-china-sea-arbitration</t>
+  </si>
+  <si>
+    <t>http://www.wallstreet-online.de/nachricht/8725144-internationale-experten-stellen-verfahren-south-china-sea-arbitration-infrage</t>
+  </si>
+  <si>
+    <t>http://www.telegraphindia.com/pressrelease/prnw/en34887.html</t>
+  </si>
+  <si>
+    <t>http://www.surveysam.com/prnewswire.html?rkey=20160629EN34887&amp;filter=3083</t>
+  </si>
+  <si>
+    <t>http://www.stocklink.no/PrNewsWireItem.aspx?id=1613239&amp;title=Internationale+Experten+stellen+das+Verfahren+der+South+China+Sea+Arbitration+infrage</t>
+  </si>
+  <si>
+    <t>http://www.pressemeldungen.com/2016/06/30/internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage-340495/</t>
+  </si>
+  <si>
+    <t>http://www.press-release.by/pr-newswire?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.co.uk/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.co.uk/news-releases/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china-585004631.html</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.se/news-releases/international-experts-question-proceedings-of-south-china-sea-arbitration-584834651.html</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.fr/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.com/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
+  </si>
+  <si>
+    <t>http://www.prnewswire.com/news-releases/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china-585004631.html</t>
+  </si>
+  <si>
+    <t>http://www.padovanews.it/speciali/immedia-press/413138-international-experts-question-proceedings-of-south-china-sea-arbitration.html</t>
+  </si>
+  <si>
+    <t>http://www.onenewspage.co.uk/prnewswire.php?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://www.onenewspage.com/prnewswire.php?rkey=20160629EN34887&amp;filter=3968</t>
+  </si>
+  <si>
+    <t>http://www.presseportal.ch/de/pm/100060286/100790153</t>
+  </si>
+  <si>
+    <t>http://www.netherlandscorporatenews.com/archive/en/2016/06/29/Y018.htm</t>
+  </si>
+  <si>
+    <t>http://mokanews.es/prensa/?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
+  </si>
+  <si>
+    <t>http://www.mediaddress.es/comunicacion/es/comunicados-de-prensa/614800/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china.html</t>
+  </si>
+  <si>
+    <t>http://www.portugalfinancialadvice.com/prnewswirespanish.html?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
+  </si>
+  <si>
+    <t>http://news.infrosoft.com/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://globalnewsweek.com/prnewswire/index.html?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://www.finanznavigator.de/fn/news_ots.php?do=detail&amp;NEWS_ID=492686</t>
+  </si>
+  <si>
+    <t>http://www.finanznachrichten.de/nachrichten-2016-06/37828494-international-experts-question-proceedings-of-south-china-sea-arbitration-008.htm</t>
+  </si>
+  <si>
+    <t>http://www.finanznachrichten.de/nachrichten-2016-06/37843885-internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage-007.htm</t>
+  </si>
+  <si>
+    <t>http://www.finanzen.net/nachricht/aktien/Internationale-Experten-stellen-das-Verfahren-der-South-China-Sea-Arbitration-infrage-4961779</t>
+  </si>
+  <si>
+    <t>http://www.finanzen.at/nachrichten/aktien/Internationale-Experten-stellen-das-Verfahren-der-South-China-Sea-Arbitration-infrage-1001280949</t>
+  </si>
+  <si>
+    <t>http://ezerin.com/pr-newswire/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://www.europapress.es/comunicados/internacional/noticia-comunicado-expertos-internacionales-cuestionan-procedimientos-arbitraje-mar-sur-china-20160630120253.html</t>
+  </si>
+  <si>
+    <t>http://erdesvan.info/noticias-de-pr-newswire/?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
+  </si>
+  <si>
+    <t>http://bolsa.diariodeleon.es/noticias-actualidad/notasDePrensa/Expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-Mar-del-Sur-de-China--SP34887--18a36ceeb2e4593a62369c272554cbdb.html</t>
+  </si>
+  <si>
+    <t>http://www.tagesspiegel.de/advertorials/ots/wuhan-university-internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage/13811054.html</t>
+  </si>
+  <si>
+    <t>http://www.creditmarket.co.uk/latest-finance-news/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://www.collaboration-technologies.co.uk/prnews.htm?rkey=20160629EN34887&amp;filter=5955</t>
+  </si>
+  <si>
+    <t>http://boxticker.com/prnewswire.html?rkey=20160629EN34887&amp;filter=5555</t>
+  </si>
+  <si>
+    <t>http://www.boursica.com/informations-communiques-bourse/lire-depeche.php1/news/195818</t>
+  </si>
+  <si>
+    <t>http://boerse-social.com/2016/06/30/internationale_experten_stellen_das_verfahren_der_south_china_sea_arbitration_infrage</t>
+  </si>
+  <si>
+    <t>https://www.boerse-go.de/nachricht/internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage,a4755672.html</t>
+  </si>
+  <si>
+    <t>http://www.belgamediasupport.be/pressrelease/detail.do?pressId=55673&amp;type=thisweek&amp;searchKey=f04975b8-3ea9-11e6-b2ae-1133c35c9bbc&amp;languageId=all&amp;pageIndex=1</t>
+  </si>
+  <si>
+    <t>http://b-live.in/prnewswire/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://assignmenteditor.com/pr-newswire-3/?rkey=20160629EN34887&amp;filter=1673</t>
+  </si>
+  <si>
+    <t>http://aladnani.com/news.html?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
+  </si>
+  <si>
+    <t>http://mx.advfn.com/p.php?pid=nmona&amp;article=71858520</t>
+  </si>
+  <si>
+    <t>http://de.advfn.com/p.php?pid=nmona&amp;article=71846988</t>
+  </si>
+  <si>
+    <t>http://fr.advfn.com/actualites/Des-experts-internationaux-emettent-des-reserves-s_71858448.html</t>
+  </si>
+  <si>
+    <t>http://www.adnkronos.com/immediapress/pr-newswire/2016/06/29/international-experts-question-proceedings-south-china-sea-arbitration_KOWOo2WyhxVnuhMnGjlOLP.html</t>
+  </si>
+  <si>
+    <t>Klout score</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
     <t>France</t>
   </si>
   <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>global</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Retweets</t>
+  </si>
+  <si>
     <t>Blog</t>
   </si>
   <si>
+    <t>Trade Publications</t>
+  </si>
+  <si>
+    <t>Newspaper</t>
+  </si>
+  <si>
+    <t>Online News Sites &amp; Other Influencers</t>
+  </si>
+  <si>
+    <t>News &amp; Information Service</t>
+  </si>
+  <si>
+    <t>Portal</t>
+  </si>
+  <si>
+    <t>Financial News Service</t>
+  </si>
+  <si>
     <t>Retail &amp; Consumer</t>
   </si>
   <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Media &amp; Information</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Tech</t>
+  </si>
+  <si>
+    <t>Business Services</t>
+  </si>
+  <si>
     <t>Not Available</t>
   </si>
   <si>
@@ -50,468 +542,6 @@
   </si>
   <si>
     <t>Des experts internationaux émettent des réserves sur la procédure d'arbitrage de la mer de Chine méridionale</t>
-  </si>
-  <si>
-    <t>EN34887</t>
-  </si>
-  <si>
-    <t>GE34887</t>
-  </si>
-  <si>
-    <t>SP34887</t>
-  </si>
-  <si>
-    <t>Tweets</t>
-  </si>
-  <si>
-    <t>Twitter Handle</t>
-  </si>
-  <si>
-    <t>Newswire IO (newswireio)</t>
-  </si>
-  <si>
-    <t>CIAR GLOBAL (CIAR_Global)</t>
-  </si>
-  <si>
-    <t>CentroIberoamericano (CIAR_Arbitraje)</t>
-  </si>
-  <si>
-    <t>Bojami Nguyen (NguyenBojami)</t>
-  </si>
-  <si>
-    <t>David Nguyen (davidvietnguyen)</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>German</t>
-  </si>
-  <si>
-    <t>Spanish</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>https://twitter.com/newswireio/statuses/748462216266059776</t>
-  </si>
-  <si>
-    <t>https://twitter.com/CIAR_Global/statuses/748829787549011968</t>
-  </si>
-  <si>
-    <t>https://twitter.com/CIAR_Arbitraje/statuses/748834819207987200</t>
-  </si>
-  <si>
-    <t>https://twitter.com/NguyenBojami/statuses/748124799306731520</t>
-  </si>
-  <si>
-    <t>https://twitter.com/davidvietnguyen/statuses/748136832228024320</t>
-  </si>
-  <si>
-    <t>wallstreet:online</t>
-  </si>
-  <si>
-    <t>Telegraph India</t>
-  </si>
-  <si>
-    <t>SurveySam.com</t>
-  </si>
-  <si>
-    <t>Stocklink</t>
-  </si>
-  <si>
-    <t>Pressemeldungen</t>
-  </si>
-  <si>
-    <t>Press-Release.by</t>
-  </si>
-  <si>
-    <t>PR Newswire UK</t>
-  </si>
-  <si>
-    <t>PR Newswire Sweden</t>
-  </si>
-  <si>
-    <t>PR Newswire France</t>
-  </si>
-  <si>
-    <t>PR Newswire</t>
-  </si>
-  <si>
-    <t>Padova News</t>
-  </si>
-  <si>
-    <t>One News Page United Kingdom Edition</t>
-  </si>
-  <si>
-    <t>One News Page Global Edition</t>
-  </si>
-  <si>
-    <t>news aktuell Switzerland</t>
-  </si>
-  <si>
-    <t>Netherlands Corporate News</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mokanews	</t>
-  </si>
-  <si>
-    <t>Mediaddress.es</t>
-  </si>
-  <si>
-    <t>Luso Financial Planning</t>
-  </si>
-  <si>
-    <t>Infrosoft</t>
-  </si>
-  <si>
-    <t>Global Newsweek</t>
-  </si>
-  <si>
-    <t>Finanznavigator</t>
-  </si>
-  <si>
-    <t>FinanzNachrichten.de (ABC New Media AG)</t>
-  </si>
-  <si>
-    <t>finanzen.net</t>
-  </si>
-  <si>
-    <t>Finanzen.at</t>
-  </si>
-  <si>
-    <t>EZERINCOM</t>
-  </si>
-  <si>
-    <t>Europa Press</t>
-  </si>
-  <si>
-    <t>ErDesvan</t>
-  </si>
-  <si>
-    <t>Diario de Leon</t>
-  </si>
-  <si>
-    <t>Der Tagesspiegel</t>
-  </si>
-  <si>
-    <t>Creditmarket.co.uk</t>
-  </si>
-  <si>
-    <t>Collaboration Technologies</t>
-  </si>
-  <si>
-    <t>BoxTicker.com</t>
-  </si>
-  <si>
-    <t>Boursica</t>
-  </si>
-  <si>
-    <t>Borse Social Network</t>
-  </si>
-  <si>
-    <t>BoerseGo</t>
-  </si>
-  <si>
-    <t>Belga Direct</t>
-  </si>
-  <si>
-    <t>B Live News</t>
-  </si>
-  <si>
-    <t>AssignmentEditor.com</t>
-  </si>
-  <si>
-    <t>Al-Adnani</t>
-  </si>
-  <si>
-    <t>ADVFN Mexico</t>
-  </si>
-  <si>
-    <t>ADVFN Germany</t>
-  </si>
-  <si>
-    <t>ADVFN France</t>
-  </si>
-  <si>
-    <t>ADN Kronos</t>
-  </si>
-  <si>
-    <t>Potential Audience</t>
-  </si>
-  <si>
-    <t>2925 followers</t>
-  </si>
-  <si>
-    <t>88 followers</t>
-  </si>
-  <si>
-    <t>64 followers</t>
-  </si>
-  <si>
-    <t>33 followers</t>
-  </si>
-  <si>
-    <t>20 followers</t>
-  </si>
-  <si>
-    <t>Published on</t>
-  </si>
-  <si>
-    <t>2016-06-30 10:37:26</t>
-  </si>
-  <si>
-    <t>2016-07-01 10:52:25</t>
-  </si>
-  <si>
-    <t>2016-07-01 11:07:26</t>
-  </si>
-  <si>
-    <t>2016-06-29 12:07:36</t>
-  </si>
-  <si>
-    <t>2016-06-29 12:52:47</t>
-  </si>
-  <si>
-    <t>http://www.wallstreet-online.de/nachricht/8721253-international-experts-question-proceedings-of-south-china-sea-arbitration</t>
-  </si>
-  <si>
-    <t>http://www.wallstreet-online.de/nachricht/8725144-internationale-experten-stellen-verfahren-south-china-sea-arbitration-infrage</t>
-  </si>
-  <si>
-    <t>http://www.telegraphindia.com/pressrelease/prnw/en34887.html</t>
-  </si>
-  <si>
-    <t>http://www.surveysam.com/prnewswire.html?rkey=20160629EN34887&amp;filter=3083</t>
-  </si>
-  <si>
-    <t>http://www.stocklink.no/PrNewsWireItem.aspx?id=1613239&amp;title=Internationale+Experten+stellen+das+Verfahren+der+South+China+Sea+Arbitration+infrage</t>
-  </si>
-  <si>
-    <t>http://www.pressemeldungen.com/2016/06/30/internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage-340495/</t>
-  </si>
-  <si>
-    <t>http://www.press-release.by/pr-newswire?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.co.uk/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.co.uk/news-releases/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china-585004631.html</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.se/news-releases/international-experts-question-proceedings-of-south-china-sea-arbitration-584834651.html</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.fr/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.com/news-releases/des-experts-internationaux-emettent-des-reserves-sur-la-procedure-darbitrage-de-la-mer-de-chine-meridionale-585003761.html</t>
-  </si>
-  <si>
-    <t>http://www.prnewswire.com/news-releases/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china-585004631.html</t>
-  </si>
-  <si>
-    <t>http://www.padovanews.it/speciali/immedia-press/413138-international-experts-question-proceedings-of-south-china-sea-arbitration.html</t>
-  </si>
-  <si>
-    <t>http://www.onenewspage.co.uk/prnewswire.php?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://www.onenewspage.com/prnewswire.php?rkey=20160629EN34887&amp;filter=3968</t>
-  </si>
-  <si>
-    <t>http://www.presseportal.ch/de/pm/100060286/100790153</t>
-  </si>
-  <si>
-    <t>http://www.netherlandscorporatenews.com/archive/en/2016/06/29/Y018.htm</t>
-  </si>
-  <si>
-    <t>http://mokanews.es/prensa/?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
-  </si>
-  <si>
-    <t>http://www.mediaddress.es/comunicacion/es/comunicados-de-prensa/614800/expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-mar-del-sur-de-china.html</t>
-  </si>
-  <si>
-    <t>http://www.portugalfinancialadvice.com/prnewswirespanish.html?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
-  </si>
-  <si>
-    <t>http://news.infrosoft.com/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://globalnewsweek.com/prnewswire/index.html?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://www.finanznavigator.de/fn/news_ots.php?do=detail&amp;NEWS_ID=492686</t>
-  </si>
-  <si>
-    <t>http://www.finanznachrichten.de/nachrichten-2016-06/37828494-international-experts-question-proceedings-of-south-china-sea-arbitration-008.htm</t>
-  </si>
-  <si>
-    <t>http://www.finanznachrichten.de/nachrichten-2016-06/37843885-internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage-007.htm</t>
-  </si>
-  <si>
-    <t>http://www.finanzen.net/nachricht/aktien/Internationale-Experten-stellen-das-Verfahren-der-South-China-Sea-Arbitration-infrage-4961779</t>
-  </si>
-  <si>
-    <t>http://www.finanzen.at/nachrichten/aktien/Internationale-Experten-stellen-das-Verfahren-der-South-China-Sea-Arbitration-infrage-1001280949</t>
-  </si>
-  <si>
-    <t>http://ezerin.com/pr-newswire/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://www.europapress.es/comunicados/internacional/noticia-comunicado-expertos-internacionales-cuestionan-procedimientos-arbitraje-mar-sur-china-20160630120253.html</t>
-  </si>
-  <si>
-    <t>http://erdesvan.info/noticias-de-pr-newswire/?doc=201606300602PR_NEWS_EURO_ND__SP34887&amp;dir=10</t>
-  </si>
-  <si>
-    <t>http://bolsa.diariodeleon.es/noticias-actualidad/notasDePrensa/Expertos-internacionales-cuestionan-los-procedimientos-de-arbitraje-del-Mar-del-Sur-de-China--SP34887--18a36ceeb2e4593a62369c272554cbdb.html</t>
-  </si>
-  <si>
-    <t>http://www.tagesspiegel.de/advertorials/ots/wuhan-university-internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage/13811054.html</t>
-  </si>
-  <si>
-    <t>http://www.creditmarket.co.uk/latest-finance-news/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://www.collaboration-technologies.co.uk/prnews.htm?rkey=20160629EN34887&amp;filter=5955</t>
-  </si>
-  <si>
-    <t>http://boxticker.com/prnewswire.html?rkey=20160629EN34887&amp;filter=5555</t>
-  </si>
-  <si>
-    <t>http://www.boursica.com/informations-communiques-bourse/lire-depeche.php1/news/195818</t>
-  </si>
-  <si>
-    <t>http://boerse-social.com/2016/06/30/internationale_experten_stellen_das_verfahren_der_south_china_sea_arbitration_infrage</t>
-  </si>
-  <si>
-    <t>https://www.boerse-go.de/nachricht/internationale-experten-stellen-das-verfahren-der-south-china-sea-arbitration-infrage,a4755672.html</t>
-  </si>
-  <si>
-    <t>http://www.belgamediasupport.be/pressrelease/detail.do?pressId=55673&amp;type=thisweek&amp;searchKey=f04975b8-3ea9-11e6-b2ae-1133c35c9bbc&amp;languageId=all&amp;pageIndex=1</t>
-  </si>
-  <si>
-    <t>http://b-live.in/prnewswire/?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://assignmenteditor.com/pr-newswire-3/?rkey=20160629EN34887&amp;filter=1673</t>
-  </si>
-  <si>
-    <t>http://aladnani.com/news.html?doc=201606290708PR_NEWS_EURO_ND__EN34887&amp;dir=2</t>
-  </si>
-  <si>
-    <t>http://mx.advfn.com/p.php?pid=nmona&amp;article=71858520</t>
-  </si>
-  <si>
-    <t>http://de.advfn.com/p.php?pid=nmona&amp;article=71846988</t>
-  </si>
-  <si>
-    <t>http://fr.advfn.com/actualites/Des-experts-internationaux-emettent-des-reserves-s_71858448.html</t>
-  </si>
-  <si>
-    <t>http://www.adnkronos.com/immediapress/pr-newswire/2016/06/29/international-experts-question-proceedings-south-china-sea-arbitration_KOWOo2WyhxVnuhMnGjlOLP.html</t>
-  </si>
-  <si>
-    <t>Klout score</t>
-  </si>
-  <si>
-    <t>37</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>34</t>
-  </si>
-  <si>
-    <t>26</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t>Germany</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
-  </si>
-  <si>
-    <t>Norway</t>
-  </si>
-  <si>
-    <t>Belarus</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>United States</t>
-  </si>
-  <si>
-    <t>Italy</t>
-  </si>
-  <si>
-    <t>global</t>
-  </si>
-  <si>
-    <t>Switzerland</t>
-  </si>
-  <si>
-    <t>Netherlands</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Portugal</t>
-  </si>
-  <si>
-    <t>Belgium</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Retweets</t>
-  </si>
-  <si>
-    <t>Trade Publications</t>
-  </si>
-  <si>
-    <t>Newspaper</t>
-  </si>
-  <si>
-    <t>Online News Sites &amp; Other Influencers</t>
-  </si>
-  <si>
-    <t>News &amp; Information Service</t>
-  </si>
-  <si>
-    <t>Portal</t>
-  </si>
-  <si>
-    <t>Financial News Service</t>
-  </si>
-  <si>
-    <t>Financial</t>
-  </si>
-  <si>
-    <t>Media &amp; Information</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Tech</t>
-  </si>
-  <si>
-    <t>Business Services</t>
   </si>
   <si>
     <t>International Experts Question Proceedings of South China Sea Arbitration</t>
@@ -936,40 +966,40 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="G2" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="H2" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="I2" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="J2" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K2" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L2" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M2" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -977,40 +1007,40 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G3" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H3" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J3">
         <v>35597</v>
       </c>
       <c r="K3" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L3" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M3" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -1018,40 +1048,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="G4" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H4" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I4" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J4">
         <v>35597</v>
       </c>
       <c r="K4" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L4" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M4" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -1059,40 +1089,40 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="I5" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J5">
         <v>13039</v>
       </c>
       <c r="K5" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L5" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M5" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:13">
@@ -1100,40 +1130,40 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G6" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I6" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M6" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:13">
@@ -1141,40 +1171,40 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="H7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I7" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J7">
         <v>1437</v>
       </c>
       <c r="K7" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L7" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M7" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1182,40 +1212,40 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="G8" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H8" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I8" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K8" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L8" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M8" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -1223,40 +1253,40 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H9" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I9" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J9" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K9" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L9" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M9" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1264,40 +1294,40 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="G10" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J10">
         <v>1117</v>
       </c>
       <c r="K10" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L10" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M10" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -1305,40 +1335,40 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="G11" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J11">
         <v>1117</v>
       </c>
       <c r="K11" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L11" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M11" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -1346,40 +1376,40 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G12" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J12" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K12" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L12" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M12" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1387,40 +1417,40 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="G13" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="H13" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I13" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J13" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K13" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L13" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M13" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1428,40 +1458,40 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G14" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I14" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J14">
         <v>181146</v>
       </c>
       <c r="K14" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L14" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M14" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1469,40 +1499,40 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E15" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G15" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H15" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J15">
         <v>181146</v>
       </c>
       <c r="K15" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L15" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M15" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1510,40 +1540,40 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G16" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H16" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J16" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K16" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L16" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M16" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1551,40 +1581,40 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G17" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H17" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I17" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J17">
         <v>786</v>
       </c>
       <c r="K17" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L17" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M17" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1592,40 +1622,40 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H18" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I18" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J18">
         <v>23333</v>
       </c>
       <c r="K18" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L18" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M18" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1633,40 +1663,40 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="G19" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I19" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J19" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K19" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L19" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M19" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1674,40 +1704,40 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G20" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H20" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I20" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J20" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K20" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L20" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M20" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -1715,40 +1745,40 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G21" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H21" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J21" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K21" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L21" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M21" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:13">
@@ -1756,40 +1786,40 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E22" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G22" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H22" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I22" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K22" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L22" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M22" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="1:13">
@@ -1797,40 +1827,40 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G23" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H23" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I23" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J23" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K23" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L23" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M23" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:13">
@@ -1838,40 +1868,40 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="G24" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I24" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="J24" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K24" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L24" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M24" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="25" spans="1:13">
@@ -1879,40 +1909,40 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G25" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I25" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J25" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K25" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L25" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M25" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="26" spans="1:13">
@@ -1920,40 +1950,40 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="G26" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H26" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I26" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J26" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K26" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L26" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M26" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="27" spans="1:13">
@@ -1961,40 +1991,40 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G27" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H27" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I27" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J27">
         <v>67785</v>
       </c>
       <c r="K27" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L27" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M27" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:13">
@@ -2002,40 +2032,40 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C28" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D28" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G28" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H28" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I28" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J28">
         <v>67785</v>
       </c>
       <c r="K28" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L28" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M28" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:13">
@@ -2043,40 +2073,40 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="E29" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G29" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H29" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I29" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J29">
         <v>178337</v>
       </c>
       <c r="K29" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L29" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M29" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:13">
@@ -2084,40 +2114,40 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E30" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G30" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H30" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I30" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J30">
         <v>12423</v>
       </c>
       <c r="K30" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L30" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M30" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:13">
@@ -2125,40 +2155,40 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E31" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G31" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I31" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J31" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K31" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L31" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M31" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="32" spans="1:13">
@@ -2166,40 +2196,40 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G32" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H32" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="I32" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J32">
         <v>202779</v>
       </c>
       <c r="K32" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L32" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M32" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:13">
@@ -2207,40 +2237,40 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C33" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="G33" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H33" t="s">
-        <v>6</v>
+        <v>159</v>
       </c>
       <c r="I33" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K33" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L33" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M33" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="34" spans="1:13">
@@ -2248,40 +2278,40 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D34" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G34" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="I34" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J34" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K34" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L34" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M34" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="35" spans="1:13">
@@ -2289,40 +2319,40 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E35" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G35" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I35" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J35">
         <v>81651</v>
       </c>
       <c r="K35" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L35" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M35" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:13">
@@ -2330,40 +2360,40 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D36" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="G36" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H36" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I36" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J36" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K36" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L36" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M36" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:13">
@@ -2371,40 +2401,40 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D37" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G37" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H37" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I37" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="J37" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K37" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L37" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M37" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:13">
@@ -2412,40 +2442,40 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G38" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H38" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I38" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="J38" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K38" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L38" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M38" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:13">
@@ -2453,40 +2483,40 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E39" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="G39" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="H39" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I39" t="s">
-        <v>163</v>
+        <v>169</v>
       </c>
       <c r="J39" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K39" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L39" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M39" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:13">
@@ -2494,40 +2524,40 @@
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E40" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G40" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H40" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="I40" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J40" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K40" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L40" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M40" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:13">
@@ -2535,40 +2565,40 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E41" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G41" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H41" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="I41" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J41">
         <v>7017</v>
       </c>
       <c r="K41" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L41" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M41" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:13">
@@ -2576,40 +2606,40 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D42" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E42" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G42" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="H42" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I42" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J42" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K42" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L42" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M42" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:13">
@@ -2617,40 +2647,40 @@
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E43" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G43" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I43" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J43" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K43" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L43" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M43" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:13">
@@ -2658,40 +2688,40 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D44" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G44" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H44" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I44" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J44" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K44" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L44" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M44" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="45" spans="1:13">
@@ -2699,40 +2729,40 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="G45" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H45" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I45" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J45" t="s">
-        <v>8</v>
+        <v>172</v>
       </c>
       <c r="K45" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L45" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M45" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:13">
@@ -2740,40 +2770,40 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E46" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G46" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="H46" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I46" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J46">
         <v>241103</v>
       </c>
       <c r="K46" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L46" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M46" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:13">
@@ -2781,40 +2811,40 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G47" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H47" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I47" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J47">
         <v>241103</v>
       </c>
       <c r="K47" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L47" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M47" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="48" spans="1:13">
@@ -2822,40 +2852,40 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E48" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="G48" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="H48" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="I48" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
       <c r="J48">
         <v>241103</v>
       </c>
       <c r="K48" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L48" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M48" t="s">
-        <v>11</v>
+        <v>175</v>
       </c>
     </row>
     <row r="49" spans="1:13">
@@ -2863,40 +2893,40 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E49" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G49" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="H49" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="I49" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="J49">
         <v>46426</v>
       </c>
       <c r="K49" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="L49" t="s">
-        <v>10</v>
+        <v>174</v>
       </c>
       <c r="M49" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="1:13">
@@ -2919,7 +2949,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="54" spans="1:13">
@@ -2932,22 +2962,22 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C55" t="s">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D55" t="s">
-        <v>74</v>
+        <v>8</v>
       </c>
       <c r="E55" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F55" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G55" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="1:13">
@@ -2955,19 +2985,19 @@
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D56" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E56" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F56" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
     </row>
     <row r="57" spans="1:13">
@@ -2975,19 +3005,19 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E57" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F57" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
     </row>
     <row r="58" spans="1:13">
@@ -2995,19 +3025,19 @@
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D58" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E58" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="F58" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:13">
@@ -3015,19 +3045,19 @@
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E59" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F59" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:13">
@@ -3035,77 +3065,76 @@
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D60" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E60" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F60" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F1" r:id="rId1"/>
-    <hyperlink ref="F2" r:id="rId2"/>
-    <hyperlink ref="F3" r:id="rId3"/>
-    <hyperlink ref="F4" r:id="rId4"/>
-    <hyperlink ref="F5" r:id="rId5"/>
-    <hyperlink ref="F6" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
-    <hyperlink ref="F8" r:id="rId8"/>
-    <hyperlink ref="F9" r:id="rId9"/>
-    <hyperlink ref="F10" r:id="rId10"/>
-    <hyperlink ref="F11" r:id="rId11"/>
-    <hyperlink ref="F12" r:id="rId12"/>
-    <hyperlink ref="F13" r:id="rId13"/>
-    <hyperlink ref="F14" r:id="rId14"/>
-    <hyperlink ref="F15" r:id="rId15"/>
-    <hyperlink ref="F16" r:id="rId16"/>
-    <hyperlink ref="F17" r:id="rId17"/>
-    <hyperlink ref="F18" r:id="rId18"/>
-    <hyperlink ref="F19" r:id="rId19"/>
-    <hyperlink ref="F20" r:id="rId20"/>
-    <hyperlink ref="F21" r:id="rId21"/>
-    <hyperlink ref="F22" r:id="rId22"/>
-    <hyperlink ref="F23" r:id="rId23"/>
-    <hyperlink ref="F24" r:id="rId24"/>
-    <hyperlink ref="F25" r:id="rId25"/>
-    <hyperlink ref="F26" r:id="rId26"/>
-    <hyperlink ref="F27" r:id="rId27"/>
-    <hyperlink ref="F28" r:id="rId28"/>
-    <hyperlink ref="F29" r:id="rId29"/>
-    <hyperlink ref="F30" r:id="rId30"/>
-    <hyperlink ref="F31" r:id="rId31"/>
-    <hyperlink ref="F32" r:id="rId32"/>
-    <hyperlink ref="F33" r:id="rId33"/>
-    <hyperlink ref="F34" r:id="rId34"/>
-    <hyperlink ref="F35" r:id="rId35"/>
-    <hyperlink ref="F36" r:id="rId36"/>
-    <hyperlink ref="F37" r:id="rId37"/>
-    <hyperlink ref="F38" r:id="rId38"/>
-    <hyperlink ref="F39" r:id="rId39"/>
-    <hyperlink ref="F40" r:id="rId40"/>
-    <hyperlink ref="F41" r:id="rId41"/>
-    <hyperlink ref="F42" r:id="rId42"/>
-    <hyperlink ref="F43" r:id="rId43"/>
-    <hyperlink ref="F44" r:id="rId44"/>
-    <hyperlink ref="F45" r:id="rId45"/>
-    <hyperlink ref="F46" r:id="rId46"/>
-    <hyperlink ref="F47" r:id="rId47"/>
-    <hyperlink ref="F48" r:id="rId48"/>
-    <hyperlink ref="F49" r:id="rId49"/>
-    <hyperlink ref="C56" r:id="rId50"/>
-    <hyperlink ref="C57" r:id="rId51"/>
-    <hyperlink ref="C58" r:id="rId52"/>
-    <hyperlink ref="C59" r:id="rId53"/>
-    <hyperlink ref="C60" r:id="rId54"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="F5" r:id="rId4"/>
+    <hyperlink ref="F6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
+    <hyperlink ref="F8" r:id="rId7"/>
+    <hyperlink ref="F9" r:id="rId8"/>
+    <hyperlink ref="F10" r:id="rId9"/>
+    <hyperlink ref="F11" r:id="rId10"/>
+    <hyperlink ref="F12" r:id="rId11"/>
+    <hyperlink ref="F13" r:id="rId12"/>
+    <hyperlink ref="F14" r:id="rId13"/>
+    <hyperlink ref="F15" r:id="rId14"/>
+    <hyperlink ref="F16" r:id="rId15"/>
+    <hyperlink ref="F17" r:id="rId16"/>
+    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F19" r:id="rId18"/>
+    <hyperlink ref="F20" r:id="rId19"/>
+    <hyperlink ref="F21" r:id="rId20"/>
+    <hyperlink ref="F22" r:id="rId21"/>
+    <hyperlink ref="F23" r:id="rId22"/>
+    <hyperlink ref="F24" r:id="rId23"/>
+    <hyperlink ref="F25" r:id="rId24"/>
+    <hyperlink ref="F26" r:id="rId25"/>
+    <hyperlink ref="F27" r:id="rId26"/>
+    <hyperlink ref="F28" r:id="rId27"/>
+    <hyperlink ref="F29" r:id="rId28"/>
+    <hyperlink ref="F30" r:id="rId29"/>
+    <hyperlink ref="F31" r:id="rId30"/>
+    <hyperlink ref="F32" r:id="rId31"/>
+    <hyperlink ref="F33" r:id="rId32"/>
+    <hyperlink ref="F34" r:id="rId33"/>
+    <hyperlink ref="F35" r:id="rId34"/>
+    <hyperlink ref="F36" r:id="rId35"/>
+    <hyperlink ref="F37" r:id="rId36"/>
+    <hyperlink ref="F38" r:id="rId37"/>
+    <hyperlink ref="F39" r:id="rId38"/>
+    <hyperlink ref="F40" r:id="rId39"/>
+    <hyperlink ref="F41" r:id="rId40"/>
+    <hyperlink ref="F42" r:id="rId41"/>
+    <hyperlink ref="F43" r:id="rId42"/>
+    <hyperlink ref="F44" r:id="rId43"/>
+    <hyperlink ref="F45" r:id="rId44"/>
+    <hyperlink ref="F46" r:id="rId45"/>
+    <hyperlink ref="F47" r:id="rId46"/>
+    <hyperlink ref="F48" r:id="rId47"/>
+    <hyperlink ref="F49" r:id="rId48"/>
+    <hyperlink ref="C56" r:id="rId49"/>
+    <hyperlink ref="C57" r:id="rId50"/>
+    <hyperlink ref="C58" r:id="rId51"/>
+    <hyperlink ref="C59" r:id="rId52"/>
+    <hyperlink ref="C60" r:id="rId53"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>